<commit_message>
Built site for MassWateR: 1.0.0.9000@a3cb459
</commit_message>
<xml_diff>
--- a/MassWateR_WQXMeta_Template.xlsx
+++ b/MassWateR_WQXMeta_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Templates for users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA038AA4-2DBE-44C9-B819-E783649C4F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE0719B-9CAE-4E5D-B009-96EFAD129DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
@@ -284,20 +284,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,17 +619,17 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="14" customWidth="1"/>
     <col min="2" max="6" width="13.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -652,19 +652,19 @@
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -672,19 +672,19 @@
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="B3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -692,19 +692,19 @@
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -712,19 +712,19 @@
       <c r="A5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -732,19 +732,19 @@
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="C6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -854,7 +854,7 @@
       <c r="C9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>